<commit_message>
reading by cell type
</commit_message>
<xml_diff>
--- a/src/main/resources/Book1.xlsx
+++ b/src/main/resources/Book1.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Title 1</t>
   </si>
@@ -88,8 +88,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,7 +374,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,8 +399,8 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
+      <c r="B3" s="1">
+        <v>4343</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -411,8 +412,8 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
+      <c r="A5" s="1">
+        <v>432.42340000000002</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
using formatter to get cell value
</commit_message>
<xml_diff>
--- a/src/main/resources/Book1.xlsx
+++ b/src/main/resources/Book1.xlsx
@@ -43,9 +43,6 @@
     <t>text3</t>
   </si>
   <si>
-    <t>text4</t>
-  </si>
-  <si>
     <t>text5</t>
   </si>
   <si>
@@ -53,6 +50,9 @@
   </si>
   <si>
     <t>text7</t>
+  </si>
+  <si>
+    <t>453,00</t>
   </si>
 </sst>
 </file>
@@ -374,7 +374,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,32 +415,32 @@
       <c r="A5" s="1">
         <v>432.42340000000002</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
getting exact location cell
</commit_message>
<xml_diff>
--- a/src/main/resources/Book1.xlsx
+++ b/src/main/resources/Book1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11865"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11865" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>Title 1</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>453,00</t>
+  </si>
+  <si>
+    <t>asd</t>
   </si>
 </sst>
 </file>
@@ -371,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,6 +446,22 @@
         <v>7</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>123</v>
+      </c>
+      <c r="B9">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -450,12 +469,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="6" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>